<commit_message>
Add part A datasheet
</commit_message>
<xml_diff>
--- a/Reproduce-Part A/datasheet.xlsx
+++ b/Reproduce-Part A/datasheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erin.cafferty/University of Bergen_onMac/Biostat II/Exam/Reproduce-Part A/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCF1560-7502-6440-9FA4-F891C89CC80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="195" windowWidth="18915" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="11800" yWindow="-20620" windowWidth="19400" windowHeight="14140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boxplotindices" sheetId="2" r:id="rId1"/>
@@ -13,26 +19,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">matrixalldataspp!$A$1:$J$1</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">matrixalldatacom!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">matrixalldatacom!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">matrixalldatacom!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">matrixalldatacom!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">matrixalldatacom!$A$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">matrixalldatacom!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">matrixalldatacom!$B$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">matrixalldatacom!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">matrixalldatacom!$A$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">matrixalldatacom!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">matrixalldatacom!$B$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">matrixalldatacom!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">matrixalldatacom!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">matrixalldatacom!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">matrixalldatacom!$A$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">matrixalldatacom!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">matrixalldatacom!$B$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">matrixalldatacom!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">matrixalldatacom!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">matrixalldatacom!$A$2:$A$13</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
@@ -575,7 +561,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,6 +580,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -624,17 +611,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,14 +627,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -687,7 +675,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -759,7 +747,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -932,16 +920,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -993,7 +981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1019,7 +1007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1045,7 +1033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1071,7 +1059,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1097,7 +1085,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1123,7 +1111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1149,7 +1137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1175,7 +1163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1201,7 +1189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1227,7 +1215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1253,7 +1241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1279,7 +1267,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1305,7 +1293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1331,7 +1319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1357,7 +1345,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1383,7 +1371,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1409,7 +1397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1435,7 +1423,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1461,7 +1449,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1487,7 +1475,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1513,7 +1501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1539,7 +1527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
@@ -1565,7 +1553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1597,20 +1585,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="28" width="11.42578125" style="1"/>
-    <col min="30" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="28" width="11.5" style="1"/>
+    <col min="29" max="29" width="10.83203125" customWidth="1"/>
+    <col min="30" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1695,11 +1684,11 @@
       <c r="AB1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1788,7 +1777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1877,7 +1866,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1966,7 +1955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2055,7 +2044,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2144,7 +2133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2233,7 +2222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2322,7 +2311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2411,7 +2400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2500,7 +2489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2589,7 +2578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2678,7 +2667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2773,16 +2762,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2792,16 +2785,16 @@
       <c r="C1" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H1" t="s">
@@ -2810,11 +2803,11 @@
       <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2846,7 +2839,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2878,7 +2871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2910,7 +2903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -2942,7 +2935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2974,7 +2967,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -3006,7 +2999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -3038,7 +3031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -3070,7 +3063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -3102,7 +3095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3134,7 +3127,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -3166,7 +3159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3198,7 +3191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3230,7 +3223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -3262,7 +3255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -3294,7 +3287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -3326,7 +3319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3358,7 +3351,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -3390,7 +3383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -3422,7 +3415,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -3454,7 +3447,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -3486,7 +3479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -3518,7 +3511,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3550,7 +3543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -3582,7 +3575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -3614,7 +3607,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -3646,7 +3639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -3678,7 +3671,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -3710,7 +3703,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3742,7 +3735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3774,7 +3767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3806,7 +3799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -3838,7 +3831,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -3870,7 +3863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -3902,7 +3895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -3934,7 +3927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -3966,7 +3959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -3998,7 +3991,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>64</v>
       </c>
@@ -4030,7 +4023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -4062,7 +4055,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -4094,7 +4087,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -4126,7 +4119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -4158,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -4190,7 +4183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -4222,7 +4215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -4254,7 +4247,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>68</v>
       </c>
@@ -4286,7 +4279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>69</v>
       </c>
@@ -4318,7 +4311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -4350,7 +4343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -4382,7 +4375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -4414,7 +4407,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -4446,7 +4439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -4478,7 +4471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -4510,7 +4503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -4542,7 +4535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -4574,7 +4567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -4606,7 +4599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -4638,7 +4631,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -4670,7 +4663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -4702,7 +4695,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -4734,7 +4727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -4766,7 +4759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -4798,7 +4791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -4830,7 +4823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -4862,7 +4855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -4894,7 +4887,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -4926,7 +4919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -4958,7 +4951,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -4990,7 +4983,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -5022,7 +5015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -5054,7 +5047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -5086,7 +5079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -5118,7 +5111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -5150,7 +5143,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -5182,7 +5175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -5214,7 +5207,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -5246,7 +5239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -5278,7 +5271,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -5310,7 +5303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -5342,7 +5335,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -5374,7 +5367,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -5406,7 +5399,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -5438,7 +5431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -5470,7 +5463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -5502,7 +5495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -5534,7 +5527,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -5566,7 +5559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -5598,7 +5591,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -5630,7 +5623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -5662,7 +5655,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -5694,7 +5687,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -5726,7 +5719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -5758,7 +5751,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -5790,7 +5783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -5822,7 +5815,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -5854,7 +5847,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -5886,7 +5879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>94</v>
       </c>
@@ -5918,7 +5911,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>94</v>
       </c>
@@ -5950,7 +5943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>95</v>
       </c>
@@ -5982,7 +5975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>95</v>
       </c>
@@ -6014,7 +6007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>96</v>
       </c>
@@ -6046,7 +6039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>96</v>
       </c>
@@ -6078,7 +6071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -6110,7 +6103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>97</v>
       </c>
@@ -6142,7 +6135,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>98</v>
       </c>
@@ -6174,7 +6167,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>98</v>
       </c>
@@ -6206,7 +6199,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -6238,7 +6231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>99</v>
       </c>
@@ -6270,7 +6263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -6302,7 +6295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>100</v>
       </c>
@@ -6334,7 +6327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>101</v>
       </c>
@@ -6366,7 +6359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>101</v>
       </c>
@@ -6398,7 +6391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>102</v>
       </c>
@@ -6430,7 +6423,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -6462,7 +6455,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>103</v>
       </c>
@@ -6494,7 +6487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>103</v>
       </c>
@@ -6526,7 +6519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -6558,7 +6551,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>104</v>
       </c>
@@ -6590,7 +6583,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>105</v>
       </c>
@@ -6622,7 +6615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>105</v>
       </c>
@@ -6654,7 +6647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>106</v>
       </c>
@@ -6686,7 +6679,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>106</v>
       </c>
@@ -6718,7 +6711,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>107</v>
       </c>
@@ -6750,7 +6743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>107</v>
       </c>
@@ -6782,7 +6775,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>108</v>
       </c>
@@ -6814,7 +6807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>108</v>
       </c>
@@ -6846,7 +6839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>109</v>
       </c>
@@ -6878,7 +6871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>109</v>
       </c>
@@ -6910,7 +6903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>110</v>
       </c>
@@ -6942,7 +6935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>110</v>
       </c>
@@ -6974,7 +6967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>111</v>
       </c>
@@ -7006,7 +6999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>111</v>
       </c>
@@ -7038,7 +7031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>112</v>
       </c>
@@ -7070,7 +7063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>112</v>
       </c>
@@ -7102,7 +7095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>113</v>
       </c>
@@ -7134,7 +7127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>113</v>
       </c>
@@ -7166,7 +7159,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>114</v>
       </c>
@@ -7198,7 +7191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>114</v>
       </c>
@@ -7230,7 +7223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>115</v>
       </c>
@@ -7262,7 +7255,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>115</v>
       </c>
@@ -7294,7 +7287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>116</v>
       </c>
@@ -7326,7 +7319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>116</v>
       </c>
@@ -7358,7 +7351,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>117</v>
       </c>
@@ -7390,7 +7383,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>117</v>
       </c>
@@ -7422,7 +7415,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>118</v>
       </c>
@@ -7454,7 +7447,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>118</v>
       </c>
@@ -7486,7 +7479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>119</v>
       </c>
@@ -7518,7 +7511,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>119</v>
       </c>
@@ -7550,7 +7543,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>120</v>
       </c>
@@ -7582,7 +7575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>120</v>
       </c>
@@ -7614,7 +7607,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>121</v>
       </c>
@@ -7646,7 +7639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>121</v>
       </c>
@@ -7678,7 +7671,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>122</v>
       </c>
@@ -7710,7 +7703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>122</v>
       </c>
@@ -7742,7 +7735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>123</v>
       </c>
@@ -7774,7 +7767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>123</v>
       </c>
@@ -7806,7 +7799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>124</v>
       </c>
@@ -7838,7 +7831,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>124</v>
       </c>
@@ -7870,7 +7863,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>125</v>
       </c>
@@ -7902,7 +7895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>125</v>
       </c>
@@ -7934,7 +7927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>126</v>
       </c>
@@ -7966,7 +7959,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>126</v>
       </c>
@@ -7998,7 +7991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>127</v>
       </c>
@@ -8030,7 +8023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>127</v>
       </c>
@@ -8062,7 +8055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>128</v>
       </c>
@@ -8094,7 +8087,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>128</v>
       </c>
@@ -8126,7 +8119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>129</v>
       </c>
@@ -8158,7 +8151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>129</v>
       </c>
@@ -8190,7 +8183,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>130</v>
       </c>
@@ -8222,7 +8215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>130</v>
       </c>
@@ -8254,7 +8247,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>131</v>
       </c>
@@ -8286,7 +8279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>131</v>
       </c>
@@ -8318,7 +8311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>132</v>
       </c>
@@ -8350,7 +8343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>132</v>
       </c>
@@ -8382,7 +8375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>133</v>
       </c>
@@ -8414,7 +8407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>133</v>
       </c>
@@ -8446,7 +8439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>134</v>
       </c>
@@ -8478,7 +8471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>134</v>
       </c>
@@ -8510,7 +8503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>135</v>
       </c>
@@ -8542,7 +8535,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>135</v>
       </c>
@@ -8574,7 +8567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>136</v>
       </c>
@@ -8606,7 +8599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>136</v>
       </c>
@@ -8638,7 +8631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>137</v>
       </c>
@@ -8670,7 +8663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>137</v>
       </c>
@@ -8702,7 +8695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>138</v>
       </c>
@@ -8734,7 +8727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>138</v>
       </c>
@@ -8766,7 +8759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>139</v>
       </c>
@@ -8798,7 +8791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>139</v>
       </c>
@@ -8830,7 +8823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>140</v>
       </c>
@@ -8862,7 +8855,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>140</v>
       </c>
@@ -8894,7 +8887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>141</v>
       </c>
@@ -8926,7 +8919,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>141</v>
       </c>
@@ -8958,7 +8951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>142</v>
       </c>
@@ -8990,7 +8983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>142</v>
       </c>
@@ -9022,7 +9015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>143</v>
       </c>
@@ -9054,7 +9047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>143</v>
       </c>
@@ -9086,7 +9079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>144</v>
       </c>
@@ -9118,7 +9111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>144</v>
       </c>
@@ -9150,7 +9143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>145</v>
       </c>
@@ -9182,7 +9175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>145</v>
       </c>
@@ -9214,7 +9207,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>146</v>
       </c>
@@ -9246,7 +9239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>146</v>
       </c>
@@ -9278,7 +9271,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>147</v>
       </c>
@@ -9310,7 +9303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>147</v>
       </c>
@@ -9342,7 +9335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>148</v>
       </c>
@@ -9374,7 +9367,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>148</v>
       </c>
@@ -9406,7 +9399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>149</v>
       </c>
@@ -9438,7 +9431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>149</v>
       </c>
@@ -9470,7 +9463,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>150</v>
       </c>
@@ -9502,7 +9495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>150</v>
       </c>
@@ -9534,7 +9527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>151</v>
       </c>
@@ -9566,7 +9559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>151</v>
       </c>
@@ -9598,7 +9591,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>152</v>
       </c>
@@ -9630,7 +9623,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>152</v>
       </c>
@@ -9662,7 +9655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>153</v>
       </c>
@@ -9694,7 +9687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>153</v>
       </c>
@@ -9726,7 +9719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>154</v>
       </c>
@@ -9758,7 +9751,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>154</v>
       </c>
@@ -9790,7 +9783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>155</v>
       </c>
@@ -9822,7 +9815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>155</v>
       </c>
@@ -9854,7 +9847,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>156</v>
       </c>
@@ -9886,7 +9879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>156</v>
       </c>
@@ -9918,7 +9911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>157</v>
       </c>
@@ -9950,7 +9943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>157</v>
       </c>
@@ -9982,7 +9975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>158</v>
       </c>
@@ -10014,7 +10007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>158</v>
       </c>
@@ -10046,7 +10039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>159</v>
       </c>
@@ -10078,7 +10071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>159</v>
       </c>
@@ -10110,7 +10103,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>160</v>
       </c>
@@ -10142,7 +10135,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>160</v>
       </c>
@@ -10174,7 +10167,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>161</v>
       </c>
@@ -10206,7 +10199,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>161</v>
       </c>
@@ -10238,7 +10231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>162</v>
       </c>
@@ -10270,7 +10263,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>162</v>
       </c>
@@ -10302,7 +10295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>163</v>
       </c>
@@ -10334,7 +10327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>163</v>
       </c>
@@ -10366,7 +10359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>164</v>
       </c>
@@ -10398,7 +10391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>164</v>
       </c>
@@ -10430,7 +10423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>165</v>
       </c>
@@ -10462,7 +10455,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>165</v>
       </c>
@@ -10494,7 +10487,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>166</v>
       </c>
@@ -10526,7 +10519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>166</v>
       </c>
@@ -10558,7 +10551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>167</v>
       </c>
@@ -10590,7 +10583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>167</v>
       </c>
@@ -10622,7 +10615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>168</v>
       </c>
@@ -10654,7 +10647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>168</v>
       </c>
@@ -10686,7 +10679,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>169</v>
       </c>
@@ -10718,7 +10711,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>169</v>
       </c>
@@ -10750,7 +10743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>170</v>
       </c>
@@ -10782,7 +10775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>170</v>
       </c>
@@ -10814,7 +10807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>171</v>
       </c>
@@ -10846,7 +10839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>171</v>
       </c>
@@ -10878,7 +10871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>172</v>
       </c>
@@ -10910,7 +10903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>172</v>
       </c>
@@ -10942,7 +10935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>173</v>
       </c>
@@ -10974,7 +10967,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>173</v>
       </c>
@@ -11006,7 +10999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>174</v>
       </c>
@@ -11038,7 +11031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>174</v>
       </c>

</xml_diff>